<commit_message>
enable the filter initially
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/filter.xlsx
+++ b/src/main/webapp/WEB-INF/books/filter.xlsx
@@ -1,15 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D4B874-DB4C-ED4B-8BA6-270ED74E9FB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="17040" windowHeight="11280"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$11</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -59,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -162,74 +170,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -241,7 +189,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -276,7 +224,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -308,9 +256,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,6 +308,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -517,18 +501,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30.75" customHeight="1" thickBot="1">
@@ -542,7 +526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" thickBot="1">
+    <row r="2" spans="1:3" ht="23" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -553,7 +537,7 @@
         <v>5122</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" thickBot="1">
+    <row r="3" spans="1:3" ht="23" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -564,7 +548,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" thickBot="1">
+    <row r="4" spans="1:3" ht="23" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -575,7 +559,7 @@
         <v>6328</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" thickBot="1">
+    <row r="5" spans="1:3" ht="23" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -586,7 +570,7 @@
         <v>6544</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" thickBot="1">
+    <row r="6" spans="1:3" ht="23" thickBot="1">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -597,7 +581,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" thickBot="1">
+    <row r="7" spans="1:3" ht="23" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -608,7 +592,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" thickBot="1">
+    <row r="8" spans="1:3" ht="23" thickBot="1">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -619,7 +603,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" thickBot="1">
+    <row r="9" spans="1:3" ht="23" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -630,7 +614,7 @@
         <v>4891</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21" thickBot="1">
+    <row r="10" spans="1:3" ht="23" thickBot="1">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -641,7 +625,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" thickBot="1">
+    <row r="11" spans="1:3" ht="23" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -653,26 +637,9 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C11" xr:uid="{8C331F0D-10C6-8E45-AC4B-8073B39977B8}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B2:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add more filter examples
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/filter.xlsx
+++ b/src/main/webapp/WEB-INF/books/filter.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D4B874-DB4C-ED4B-8BA6-270ED74E9FB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CB1099-F96B-0A48-8C54-1F53A5B1B5EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="simple" sheetId="1" r:id="rId1"/>
+    <sheet name="monthly report" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'monthly report'!$A$3:$F$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">simple!$A$1:$C$11</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Type</t>
   </si>
@@ -62,13 +64,40 @@
   </si>
   <si>
     <t>Jacob</t>
+  </si>
+  <si>
+    <t>Cape Company Monthly Report</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Customer No.</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Monthly Profit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quarterly Profit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+  </numFmts>
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,8 +125,49 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF363636"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.89999084444715716"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,8 +186,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5E8E3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE3FCFA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC3C5E5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8BBCC7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -145,13 +245,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="3" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -164,9 +275,34 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="9" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="9" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="9" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Heading 4" xfId="1" builtinId="19"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{9F5F6A9B-4F87-E048-A461-A0D03B30BB07}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -642,4 +778,350 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41AF06C-CFE2-4342-B448-F3F6C5D0B57D}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="15" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="24" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" ht="21" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" customHeight="1">
+      <c r="A4" s="12">
+        <v>42384</v>
+      </c>
+      <c r="B4" s="13">
+        <v>13</v>
+      </c>
+      <c r="C4" s="14">
+        <v>89500</v>
+      </c>
+      <c r="D4" s="14">
+        <v>62600</v>
+      </c>
+      <c r="E4" s="15">
+        <f>C4-D4</f>
+        <v>26900</v>
+      </c>
+      <c r="F4" s="16">
+        <f>E4</f>
+        <v>26900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18" customHeight="1">
+      <c r="A5" s="12">
+        <v>42415</v>
+      </c>
+      <c r="B5" s="13">
+        <v>19</v>
+      </c>
+      <c r="C5" s="14">
+        <v>100500</v>
+      </c>
+      <c r="D5" s="14">
+        <v>60300</v>
+      </c>
+      <c r="E5" s="15">
+        <f t="shared" ref="E5:E15" si="0">C5-D5</f>
+        <v>40200</v>
+      </c>
+      <c r="F5" s="16">
+        <f>E4+E5</f>
+        <v>67100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" customHeight="1">
+      <c r="A6" s="12">
+        <v>42444</v>
+      </c>
+      <c r="B6" s="13">
+        <v>25</v>
+      </c>
+      <c r="C6" s="14">
+        <v>119200</v>
+      </c>
+      <c r="D6" s="14">
+        <v>27800</v>
+      </c>
+      <c r="E6" s="15">
+        <f t="shared" si="0"/>
+        <v>91400</v>
+      </c>
+      <c r="F6" s="16">
+        <f>E4+E5+E6</f>
+        <v>158500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18" customHeight="1">
+      <c r="A7" s="12">
+        <v>42475</v>
+      </c>
+      <c r="B7" s="13">
+        <v>22</v>
+      </c>
+      <c r="C7" s="14">
+        <v>115900</v>
+      </c>
+      <c r="D7" s="14">
+        <v>79600</v>
+      </c>
+      <c r="E7" s="15">
+        <f>C7-D7</f>
+        <v>36300</v>
+      </c>
+      <c r="F7" s="17">
+        <f>E7</f>
+        <v>36300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18" customHeight="1">
+      <c r="A8" s="12">
+        <v>42505</v>
+      </c>
+      <c r="B8" s="13">
+        <v>28</v>
+      </c>
+      <c r="C8" s="14">
+        <v>123700</v>
+      </c>
+      <c r="D8" s="14">
+        <v>84000</v>
+      </c>
+      <c r="E8" s="15">
+        <f t="shared" si="0"/>
+        <v>39700</v>
+      </c>
+      <c r="F8" s="17">
+        <f>E7+E8</f>
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18" customHeight="1">
+      <c r="A9" s="12">
+        <v>42536</v>
+      </c>
+      <c r="B9" s="13">
+        <v>35</v>
+      </c>
+      <c r="C9" s="14">
+        <v>129300</v>
+      </c>
+      <c r="D9" s="14">
+        <v>83100</v>
+      </c>
+      <c r="E9" s="15">
+        <f t="shared" si="0"/>
+        <v>46200</v>
+      </c>
+      <c r="F9" s="17">
+        <f>E7+E8+E9</f>
+        <v>122200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18" customHeight="1">
+      <c r="A10" s="12">
+        <v>42566</v>
+      </c>
+      <c r="B10" s="13">
+        <v>20</v>
+      </c>
+      <c r="C10" s="14">
+        <v>110700</v>
+      </c>
+      <c r="D10" s="14">
+        <v>77300</v>
+      </c>
+      <c r="E10" s="15">
+        <f t="shared" si="0"/>
+        <v>33400</v>
+      </c>
+      <c r="F10" s="18">
+        <f>E10</f>
+        <v>33400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18" customHeight="1">
+      <c r="A11" s="12">
+        <v>42597</v>
+      </c>
+      <c r="B11" s="13">
+        <v>31</v>
+      </c>
+      <c r="C11" s="14">
+        <v>125100</v>
+      </c>
+      <c r="D11" s="14">
+        <v>85500</v>
+      </c>
+      <c r="E11" s="15">
+        <f t="shared" si="0"/>
+        <v>39600</v>
+      </c>
+      <c r="F11" s="18">
+        <f>E10+E11</f>
+        <v>73000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18" customHeight="1">
+      <c r="A12" s="12">
+        <v>42628</v>
+      </c>
+      <c r="B12" s="13">
+        <v>27</v>
+      </c>
+      <c r="C12" s="14">
+        <v>120100</v>
+      </c>
+      <c r="D12" s="14">
+        <v>78900</v>
+      </c>
+      <c r="E12" s="15">
+        <f t="shared" si="0"/>
+        <v>41200</v>
+      </c>
+      <c r="F12" s="18">
+        <f>E10+E11+E12</f>
+        <v>114200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18" customHeight="1">
+      <c r="A13" s="12">
+        <v>42658</v>
+      </c>
+      <c r="B13" s="13">
+        <v>24</v>
+      </c>
+      <c r="C13" s="14">
+        <v>118400</v>
+      </c>
+      <c r="D13" s="14">
+        <v>91000</v>
+      </c>
+      <c r="E13" s="15">
+        <f t="shared" si="0"/>
+        <v>27400</v>
+      </c>
+      <c r="F13" s="19">
+        <f>E13</f>
+        <v>27400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18" customHeight="1">
+      <c r="A14" s="12">
+        <v>42689</v>
+      </c>
+      <c r="B14" s="13">
+        <v>19</v>
+      </c>
+      <c r="C14" s="14">
+        <v>100300</v>
+      </c>
+      <c r="D14" s="14">
+        <v>65100</v>
+      </c>
+      <c r="E14" s="15">
+        <f t="shared" si="0"/>
+        <v>35200</v>
+      </c>
+      <c r="F14" s="19">
+        <f>E13+E14</f>
+        <v>62600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18" customHeight="1">
+      <c r="A15" s="12">
+        <v>42719</v>
+      </c>
+      <c r="B15" s="13">
+        <v>17</v>
+      </c>
+      <c r="C15" s="14">
+        <v>94200</v>
+      </c>
+      <c r="D15" s="14">
+        <v>65800</v>
+      </c>
+      <c r="E15" s="15">
+        <f t="shared" si="0"/>
+        <v>28400</v>
+      </c>
+      <c r="F15" s="19">
+        <f>E13+E14+E15</f>
+        <v>91000</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:F15" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C4:C15">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FFFF7128"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L11" xr:uid="{BF0AF503-C80C-B645-8E85-C7AAA07639C8}">
+      <formula1>$N$11</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>